<commit_message>
practise and other files
</commit_message>
<xml_diff>
--- a/Resources/cheatcodes.xlsx
+++ b/Resources/cheatcodes.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="173">
   <si>
     <t>SN</t>
   </si>
@@ -633,6 +633,139 @@
   <si>
     <t>provides what is the structure of table</t>
   </si>
+  <si>
+    <t>pd.read_csv("Path of csv file")</t>
+  </si>
+  <si>
+    <t>reading data from csv file</t>
+  </si>
+  <si>
+    <t>pd.read_csv(path, header =None)</t>
+  </si>
+  <si>
+    <t>to do not read 1st row as column header</t>
+  </si>
+  <si>
+    <t>pd.read_csv(filepath, sep=',', header='infer')</t>
+  </si>
+  <si>
+    <t>pd.read_csv(filepath, delimiter='|', header='None, index_col = 0)</t>
+  </si>
+  <si>
+    <t>if we donot want index column by default</t>
+  </si>
+  <si>
+    <t>dataframe.columns</t>
+  </si>
+  <si>
+    <t>to check which all column are present in df</t>
+  </si>
+  <si>
+    <t>dataframe.columns["col_name1", "col_name2]</t>
+  </si>
+  <si>
+    <t>cars.columns = ["Country_code", "Region", "Country"]</t>
+  </si>
+  <si>
+    <t>to rename the column name of the dataframe</t>
+  </si>
+  <si>
+    <t>dataframe.index</t>
+  </si>
+  <si>
+    <t>cars.index, o/p = RangeIndex(start=0, stop=8, step=1)</t>
+  </si>
+  <si>
+    <t>to get row starting number, ending num and step</t>
+  </si>
+  <si>
+    <t>dataframe.index.name = "Provide name"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">cars.index.name = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Country_code"</t>
+    </r>
+  </si>
+  <si>
+    <t>to rename the column name</t>
+  </si>
+  <si>
+    <t>dataframe.set_index([col1,col2],inplace=True)</t>
+  </si>
+  <si>
+    <t>this is set index using existing column, inplace=True will replace the original dataframe</t>
+  </si>
+  <si>
+    <t>dataframe.to_csv(Path)</t>
+  </si>
+  <si>
+    <t>dataframe.head()</t>
+  </si>
+  <si>
+    <t>First five rows</t>
+  </si>
+  <si>
+    <t>dataframe.tail()</t>
+  </si>
+  <si>
+    <t>Last five rows</t>
+  </si>
+  <si>
+    <t>dataframe.info()</t>
+  </si>
+  <si>
+    <t>displays the information of the dataframe</t>
+  </si>
+  <si>
+    <t>dataframe.describe()</t>
+  </si>
+  <si>
+    <t>displays the statistical information of dataframe</t>
+  </si>
+  <si>
+    <t>COLUMN INDEXING</t>
+  </si>
+  <si>
+    <t>dataframe["required col"]</t>
+  </si>
+  <si>
+    <t>gives the value of sales against the index</t>
+  </si>
+  <si>
+    <t>type(dataframe["required_col"])</t>
+  </si>
+  <si>
+    <t>dataframe[[col1,col2]]</t>
+  </si>
+  <si>
+    <t>dataframe.loc["label"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">df.loc[1] , df.loc[[0, 1]],df.loc[:, "Age"],df.loc[1, "Score"] ,df.loc[0:1], df.loc[df["Age"] &gt; 25]
+</t>
+  </si>
+  <si>
+    <t>its label based. to use when you know the row/column names.</t>
+  </si>
+  <si>
+    <t>dataframe.iloc["position"]</t>
+  </si>
+  <si>
+    <t>df.iloc[1] , df.iloc[0:2], df.iloc[:, 1], df.iloc[1, 2],df.iloc[0:2, 0:2]</t>
+  </si>
+  <si>
+    <t>its position based. to use when when you only know the row/column positions.</t>
+  </si>
 </sst>
 </file>
 
@@ -644,7 +777,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -827,6 +960,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color rgb="FFA31515"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Calibri"/>
@@ -847,12 +987,30 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1191,7 +1349,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1215,16 +1373,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1233,78 +1391,66 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1314,8 +1460,20 @@
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1325,13 +1483,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1340,7 +1516,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1881,7 +2057,7 @@
   <sheetPr/>
   <dimension ref="B3:E66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A26" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1972,7 +2148,7 @@
       <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="2">
@@ -2036,7 +2212,7 @@
       <c r="B14" s="2">
         <v>11</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="9" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -2047,10 +2223,10 @@
       <c r="B15" s="2">
         <v>12</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="2" t="s">
@@ -2075,10 +2251,10 @@
       <c r="B17" s="2">
         <v>14</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="10" t="s">
         <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -2144,7 +2320,7 @@
       <c r="B23" s="2">
         <v>20</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E23" s="2" t="s">
@@ -2199,7 +2375,7 @@
       <c r="B28" s="2">
         <v>25</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="9" t="s">
         <v>55</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -2273,7 +2449,7 @@
       <c r="B35" s="2">
         <v>32</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="12" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2295,7 +2471,7 @@
       <c r="B37" s="2">
         <v>34</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="9" t="s">
         <v>23</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2309,10 +2485,10 @@
       <c r="B38" s="2">
         <v>35</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D38" s="13">
         <v>81.26</v>
       </c>
       <c r="E38" s="2" t="s">
@@ -2323,7 +2499,7 @@
       <c r="B39" s="2">
         <v>36</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D39" s="2" t="s">
@@ -2395,11 +2571,11 @@
       </c>
     </row>
     <row r="48" spans="3:5">
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
     </row>
     <row r="49" ht="17" spans="2:5">
       <c r="B49" s="2">
@@ -2458,11 +2634,11 @@
       </c>
     </row>
     <row r="54" spans="3:5">
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
     </row>
     <row r="55" spans="2:5">
       <c r="B55" s="2">
@@ -2575,7 +2751,7 @@
       </c>
     </row>
     <row r="66" spans="2:2">
-      <c r="B66" s="9"/>
+      <c r="B66" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2586,18 +2762,19 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B4:E9"/>
+  <dimension ref="B4:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="34.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55.6015625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="44.2734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="3.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.90625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="89.8125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -2656,9 +2833,206 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:5">
       <c r="B9" s="1">
         <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3">
+      <c r="B11" s="1">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" ht="34" spans="2:5">
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="1">
+        <v>6</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="1">
+        <v>7</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="16" ht="17" spans="2:5">
+      <c r="B16" s="1">
+        <v>9</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" ht="34" spans="2:5">
+      <c r="B17" s="1">
+        <v>10</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" s="1">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="1">
+        <v>12</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="1">
+        <v>13</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="B21" s="1">
+        <v>14</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="1">
+        <v>15</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5">
+      <c r="C25" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="28" ht="51" spans="3:5">
+      <c r="C28" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="29" ht="34" spans="3:5">
+      <c r="C29" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>